<commit_message>
Tensions d'alim precisees. Ajout de l explication de l assymetrie (parite) de CAN
</commit_message>
<xml_diff>
--- a/AD_DA/ANNA.xlsx
+++ b/AD_DA/ANNA.xlsx
@@ -287,86 +287,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="141414"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FAFAFA"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -645,11 +577,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1205,6 +1137,10 @@
       <c r="I26">
         <f>AVERAGE(G14:G26)</f>
         <v>1.93076923076923E-2</v>
+      </c>
+      <c r="K26">
+        <f>SUM(K7:K14)</f>
+        <v>-5.0109999999999992</v>
       </c>
     </row>
     <row r="28" spans="3:13">
@@ -1639,7 +1575,7 @@
       <selection activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="5:11">
       <c r="E2" t="s">
@@ -2951,7 +2887,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>